<commit_message>
reproduce figures; bug fix
</commit_message>
<xml_diff>
--- a/data/processed/vignettes20_triage_prediction_agg_dichotomized.xlsx
+++ b/data/processed/vignettes20_triage_prediction_agg_dichotomized.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -50,7 +50,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin"/>
@@ -522,7 +521,7 @@
         <v>10</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7580076270745105</v>
+        <v>0.7580076270745104</v>
       </c>
     </row>
     <row r="3">
@@ -921,7 +920,7 @@
         <v>9</v>
       </c>
       <c r="G17" t="n">
-        <v>0.638399133100143</v>
+        <v>0.6383991331001428</v>
       </c>
     </row>
     <row r="18">
@@ -988,7 +987,7 @@
         <v>5</v>
       </c>
       <c r="G20" t="n">
-        <v>0.5541080956331033</v>
+        <v>0.5541080956331034</v>
       </c>
     </row>
     <row r="21">
@@ -1204,7 +1203,7 @@
         <v>10</v>
       </c>
       <c r="G28" t="n">
-        <v>0.5537387794106072</v>
+        <v>0.5537387794106073</v>
       </c>
     </row>
     <row r="29">
@@ -1254,7 +1253,7 @@
         <v>5</v>
       </c>
       <c r="G30" t="n">
-        <v>0.4279004159092213</v>
+        <v>0.4279004159092212</v>
       </c>
     </row>
     <row r="31">
@@ -1304,7 +1303,7 @@
         <v>6</v>
       </c>
       <c r="G32" t="n">
-        <v>0.6314309414291884</v>
+        <v>0.6314309414291885</v>
       </c>
     </row>
     <row r="33">
@@ -1370,7 +1369,7 @@
         <v>10</v>
       </c>
       <c r="G34" t="n">
-        <v>0.7384428142999222</v>
+        <v>0.7384428142999221</v>
       </c>
     </row>
     <row r="35">
@@ -1503,7 +1502,7 @@
         <v>10</v>
       </c>
       <c r="G39" t="n">
-        <v>0.6109300864320387</v>
+        <v>0.6109300864320386</v>
       </c>
     </row>
     <row r="40">
@@ -1984,7 +1983,7 @@
         <v>10</v>
       </c>
       <c r="G56" t="n">
-        <v>0.5767399415904715</v>
+        <v>0.5767399415904714</v>
       </c>
     </row>
     <row r="57">
@@ -2063,7 +2062,7 @@
         <v>10</v>
       </c>
       <c r="G59" t="n">
-        <v>0.5779356764064599</v>
+        <v>0.5779356764064598</v>
       </c>
     </row>
     <row r="60">
@@ -2205,7 +2204,7 @@
         <v>5</v>
       </c>
       <c r="G65" t="n">
-        <v>0.6499372091524572</v>
+        <v>0.6499372091524573</v>
       </c>
     </row>
     <row r="66">
@@ -2297,7 +2296,7 @@
         <v>5</v>
       </c>
       <c r="G69" t="n">
-        <v>0.5212613325169834</v>
+        <v>0.5212613325169835</v>
       </c>
     </row>
     <row r="70">
@@ -2363,7 +2362,7 @@
         <v>7</v>
       </c>
       <c r="G71" t="n">
-        <v>0.5616047282379284</v>
+        <v>0.5616047282379283</v>
       </c>
     </row>
     <row r="72">
@@ -2413,7 +2412,7 @@
         <v>10</v>
       </c>
       <c r="G73" t="n">
-        <v>0.6611188839464232</v>
+        <v>0.661118883946423</v>
       </c>
     </row>
     <row r="74">

</xml_diff>